<commit_message>
Some forgotten commits and updates
</commit_message>
<xml_diff>
--- a/variant/SSI_delta_2021_07_06.xlsx
+++ b/variant/SSI_delta_2021_07_06.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Prøvedato</t>
   </si>
@@ -43,13 +43,118 @@
   </si>
   <si>
     <t>Deltavariant i pct. af Variant-PCR test</t>
+  </si>
+  <si>
+    <t>97,50</t>
+  </si>
+  <si>
+    <t>96,88</t>
+  </si>
+  <si>
+    <t>97,05</t>
+  </si>
+  <si>
+    <t>96,17</t>
+  </si>
+  <si>
+    <t>97,00</t>
+  </si>
+  <si>
+    <t>95,97</t>
+  </si>
+  <si>
+    <t>97,14</t>
+  </si>
+  <si>
+    <t>95,88</t>
+  </si>
+  <si>
+    <t>96,70</t>
+  </si>
+  <si>
+    <t>96,02</t>
+  </si>
+  <si>
+    <t>93,63</t>
+  </si>
+  <si>
+    <t>97,65</t>
+  </si>
+  <si>
+    <t>96,51</t>
+  </si>
+  <si>
+    <t>97,26</t>
+  </si>
+  <si>
+    <t>96,89</t>
+  </si>
+  <si>
+    <t>96,12</t>
+  </si>
+  <si>
+    <t>95,61</t>
+  </si>
+  <si>
+    <t>94,12</t>
+  </si>
+  <si>
+    <t>96,14</t>
+  </si>
+  <si>
+    <t>95,51</t>
+  </si>
+  <si>
+    <t>92,10</t>
+  </si>
+  <si>
+    <t>93,55</t>
+  </si>
+  <si>
+    <t>92,57</t>
+  </si>
+  <si>
+    <t>92,46</t>
+  </si>
+  <si>
+    <t>90,80</t>
+  </si>
+  <si>
+    <t>92,66</t>
+  </si>
+  <si>
+    <t>90,31</t>
+  </si>
+  <si>
+    <t>88,45</t>
+  </si>
+  <si>
+    <t>89,29</t>
+  </si>
+  <si>
+    <t>84,08</t>
+  </si>
+  <si>
+    <t>78,23</t>
+  </si>
+  <si>
+    <t>71,01</t>
+  </si>
+  <si>
+    <t>77,00</t>
+  </si>
+  <si>
+    <t>67,68</t>
+  </si>
+  <si>
+    <t>56,43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +188,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="AlbanyAMT"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -176,11 +286,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -211,6 +336,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -493,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -504,7 +635,7 @@
     <col min="1" max="6" width="19.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -524,683 +655,1383 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>44416</v>
+      </c>
+      <c r="B2" s="13">
+        <v>840</v>
+      </c>
+      <c r="C2" s="13">
+        <v>819</v>
+      </c>
+      <c r="D2" s="13">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <v>11</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>44415</v>
+      </c>
+      <c r="B3" s="13">
+        <v>866</v>
+      </c>
+      <c r="C3" s="13">
+        <v>839</v>
+      </c>
+      <c r="D3" s="13">
+        <v>22</v>
+      </c>
+      <c r="E3" s="13">
+        <v>5</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>44414</v>
+      </c>
+      <c r="B4" s="13">
+        <v>949</v>
+      </c>
+      <c r="C4" s="13">
+        <v>921</v>
+      </c>
+      <c r="D4" s="13">
+        <v>23</v>
+      </c>
+      <c r="E4" s="13">
+        <v>5</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>44413</v>
+      </c>
+      <c r="B5" s="13">
+        <v>967</v>
+      </c>
+      <c r="C5" s="13">
+        <v>930</v>
+      </c>
+      <c r="D5" s="13">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13">
+        <v>8</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>44412</v>
+      </c>
+      <c r="B6" s="13">
+        <v>932</v>
+      </c>
+      <c r="C6" s="13">
+        <v>904</v>
+      </c>
+      <c r="D6" s="13">
+        <v>18</v>
+      </c>
+      <c r="E6" s="13">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>44411</v>
+      </c>
+      <c r="B7" s="13">
+        <v>919</v>
+      </c>
+      <c r="C7" s="13">
+        <v>882</v>
+      </c>
+      <c r="D7" s="13">
+        <v>31</v>
+      </c>
+      <c r="E7" s="13">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>44410</v>
+      </c>
+      <c r="B8" s="13">
+        <v>945</v>
+      </c>
+      <c r="C8" s="13">
+        <v>918</v>
+      </c>
+      <c r="D8" s="13">
+        <v>23</v>
+      </c>
+      <c r="E8" s="13">
+        <v>4</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>44409</v>
+      </c>
+      <c r="B9" s="13">
+        <v>899</v>
+      </c>
+      <c r="C9" s="13">
+        <v>862</v>
+      </c>
+      <c r="D9" s="13">
+        <v>22</v>
+      </c>
+      <c r="E9" s="13">
+        <v>15</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>44408</v>
+      </c>
+      <c r="B10" s="13">
+        <v>789</v>
+      </c>
+      <c r="C10" s="13">
+        <v>763</v>
+      </c>
+      <c r="D10" s="13">
+        <v>18</v>
+      </c>
+      <c r="E10" s="13">
+        <v>8</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>44407</v>
+      </c>
+      <c r="B11" s="13">
+        <v>879</v>
+      </c>
+      <c r="C11" s="13">
+        <v>844</v>
+      </c>
+      <c r="D11" s="13">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13">
+        <v>8</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>44406</v>
+      </c>
+      <c r="B12" s="13">
+        <v>911</v>
+      </c>
+      <c r="C12" s="13">
+        <v>853</v>
+      </c>
+      <c r="D12" s="13">
+        <v>49</v>
+      </c>
+      <c r="E12" s="13">
+        <v>9</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>44405</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1023</v>
+      </c>
+      <c r="C13" s="13">
+        <v>999</v>
+      </c>
+      <c r="D13" s="13">
+        <v>18</v>
+      </c>
+      <c r="E13" s="13">
+        <v>6</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>44404</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1003</v>
+      </c>
+      <c r="C14" s="13">
+        <v>968</v>
+      </c>
+      <c r="D14" s="13">
+        <v>18</v>
+      </c>
+      <c r="E14" s="13">
+        <v>17</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>44403</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1060</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1031</v>
+      </c>
+      <c r="D15" s="13">
+        <v>18</v>
+      </c>
+      <c r="E15" s="13">
+        <v>11</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>44402</v>
+      </c>
+      <c r="B16" s="13">
+        <v>805</v>
+      </c>
+      <c r="C16" s="13">
+        <v>780</v>
+      </c>
+      <c r="D16" s="13">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13">
+        <v>13</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>44401</v>
+      </c>
+      <c r="B17" s="13">
+        <v>670</v>
+      </c>
+      <c r="C17" s="13">
+        <v>644</v>
+      </c>
+      <c r="D17" s="13">
+        <v>10</v>
+      </c>
+      <c r="E17" s="13">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>44400</v>
+      </c>
+      <c r="B18" s="13">
+        <v>774</v>
+      </c>
+      <c r="C18" s="13">
+        <v>740</v>
+      </c>
+      <c r="D18" s="13">
+        <v>20</v>
+      </c>
+      <c r="E18" s="13">
+        <v>14</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>44399</v>
+      </c>
+      <c r="B19" s="13">
+        <v>748</v>
+      </c>
+      <c r="C19" s="13">
+        <v>704</v>
+      </c>
+      <c r="D19" s="13">
+        <v>18</v>
+      </c>
+      <c r="E19" s="13">
+        <v>26</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>44398</v>
+      </c>
+      <c r="B20" s="13">
+        <v>854</v>
+      </c>
+      <c r="C20" s="13">
+        <v>821</v>
+      </c>
+      <c r="D20" s="13">
+        <v>9</v>
+      </c>
+      <c r="E20" s="13">
+        <v>24</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>44397</v>
+      </c>
+      <c r="B21" s="13">
+        <v>868</v>
+      </c>
+      <c r="C21" s="13">
+        <v>829</v>
+      </c>
+      <c r="D21" s="13">
+        <v>10</v>
+      </c>
+      <c r="E21" s="13">
+        <v>29</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>44396</v>
+      </c>
+      <c r="B22" s="13">
+        <v>886</v>
+      </c>
+      <c r="C22" s="13">
+        <v>816</v>
+      </c>
+      <c r="D22" s="13">
+        <v>20</v>
+      </c>
+      <c r="E22" s="13">
+        <v>50</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44395</v>
+      </c>
+      <c r="B23" s="13">
+        <v>775</v>
+      </c>
+      <c r="C23" s="13">
+        <v>725</v>
+      </c>
+      <c r="D23" s="13">
+        <v>10</v>
+      </c>
+      <c r="E23" s="13">
+        <v>40</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44394</v>
+      </c>
+      <c r="B24" s="13">
+        <v>834</v>
+      </c>
+      <c r="C24" s="13">
+        <v>772</v>
+      </c>
+      <c r="D24" s="13">
+        <v>15</v>
+      </c>
+      <c r="E24" s="13">
+        <v>47</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>44393</v>
+      </c>
+      <c r="B25" s="13">
+        <v>862</v>
+      </c>
+      <c r="C25" s="13">
+        <v>797</v>
+      </c>
+      <c r="D25" s="13">
+        <v>16</v>
+      </c>
+      <c r="E25" s="13">
+        <v>49</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>44392</v>
+      </c>
+      <c r="B26" s="13">
+        <v>1087</v>
+      </c>
+      <c r="C26" s="13">
+        <v>987</v>
+      </c>
+      <c r="D26" s="13">
+        <v>20</v>
+      </c>
+      <c r="E26" s="13">
+        <v>80</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>44391</v>
+      </c>
+      <c r="B27" s="13">
+        <v>1240</v>
+      </c>
+      <c r="C27" s="13">
+        <v>1149</v>
+      </c>
+      <c r="D27" s="13">
+        <v>21</v>
+      </c>
+      <c r="E27" s="13">
+        <v>70</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>44390</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1239</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1119</v>
+      </c>
+      <c r="D28" s="13">
+        <v>18</v>
+      </c>
+      <c r="E28" s="13">
+        <v>102</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>44389</v>
+      </c>
+      <c r="B29" s="13">
+        <v>1134</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1003</v>
+      </c>
+      <c r="D29" s="13">
+        <v>28</v>
+      </c>
+      <c r="E29" s="13">
+        <v>103</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>44388</v>
+      </c>
+      <c r="B30" s="13">
+        <v>962</v>
+      </c>
+      <c r="C30" s="13">
+        <v>859</v>
+      </c>
+      <c r="D30" s="13">
+        <v>20</v>
+      </c>
+      <c r="E30" s="13">
+        <v>83</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>44387</v>
+      </c>
+      <c r="B31" s="13">
+        <v>622</v>
+      </c>
+      <c r="C31" s="13">
+        <v>523</v>
+      </c>
+      <c r="D31" s="13">
+        <v>12</v>
+      </c>
+      <c r="E31" s="13">
+        <v>87</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>44386</v>
+      </c>
+      <c r="B32" s="13">
+        <v>588</v>
+      </c>
+      <c r="C32" s="13">
+        <v>460</v>
+      </c>
+      <c r="D32" s="13">
+        <v>28</v>
+      </c>
+      <c r="E32" s="13">
+        <v>100</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>44385</v>
+      </c>
+      <c r="B33" s="13">
+        <v>583</v>
+      </c>
+      <c r="C33" s="13">
+        <v>414</v>
+      </c>
+      <c r="D33" s="13">
+        <v>78</v>
+      </c>
+      <c r="E33" s="13">
+        <v>91</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>44384</v>
+      </c>
+      <c r="B34" s="13">
+        <v>626</v>
+      </c>
+      <c r="C34" s="13">
+        <v>482</v>
+      </c>
+      <c r="D34" s="13">
+        <v>76</v>
+      </c>
+      <c r="E34" s="13">
+        <v>68</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>44383</v>
+      </c>
+      <c r="B35" s="13">
+        <v>659</v>
+      </c>
+      <c r="C35" s="13">
+        <v>446</v>
+      </c>
+      <c r="D35" s="13">
+        <v>132</v>
+      </c>
+      <c r="E35" s="13">
+        <v>81</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>44382</v>
+      </c>
+      <c r="B36" s="13">
+        <v>677</v>
+      </c>
+      <c r="C36" s="13">
+        <v>382</v>
+      </c>
+      <c r="D36" s="13">
+        <v>255</v>
+      </c>
+      <c r="E36" s="13">
+        <v>40</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
         <v>44381</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B37" s="11">
         <v>405</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C37" s="11">
         <v>293</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D37" s="11">
         <v>63</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E37" s="11">
         <v>49</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F37" s="11">
         <v>72.349999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="38" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>44380</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B38" s="3">
         <v>372</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C38" s="3">
         <v>243</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D38" s="3">
         <v>83</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E38" s="3">
         <v>46</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F38" s="3">
         <v>65.319999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="39" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>44379</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B39" s="3">
         <v>395</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C39" s="3">
         <v>245</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D39" s="3">
         <v>94</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E39" s="3">
         <v>56</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F39" s="3">
         <v>62.03</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="40" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>44378</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B40" s="3">
         <v>418</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C40" s="3">
         <v>276</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D40" s="3">
         <v>77</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E40" s="3">
         <v>65</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F40" s="3">
         <v>66.03</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="41" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>44377</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B41" s="3">
         <v>502</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C41" s="3">
         <v>299</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D41" s="3">
         <v>123</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E41" s="3">
         <v>80</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F41" s="3">
         <v>59.56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="42" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>44376</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B42" s="3">
         <v>399</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C42" s="3">
         <v>214</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D42" s="3">
         <v>94</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E42" s="3">
         <v>91</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F42" s="3">
         <v>53.63</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="43" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>44375</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B43" s="3">
         <v>300</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C43" s="3">
         <v>154</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D43" s="3">
         <v>79</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E43" s="3">
         <v>67</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F43" s="3">
         <v>51.33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="44" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>44374</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B44" s="3">
         <v>195</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C44" s="3">
         <v>74</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D44" s="3">
         <v>62</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E44" s="3">
         <v>59</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F44" s="3">
         <v>37.950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="45" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>44373</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B45" s="3">
         <v>154</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C45" s="3">
         <v>55</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D45" s="3">
         <v>60</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E45" s="3">
         <v>39</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F45" s="3">
         <v>35.71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="46" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>44372</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B46" s="3">
         <v>206</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C46" s="3">
         <v>59</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D46" s="3">
         <v>72</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E46" s="3">
         <v>75</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F46" s="3">
         <v>28.64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="47" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
         <v>44371</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B47" s="3">
         <v>217</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C47" s="3">
         <v>68</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D47" s="3">
         <v>96</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E47" s="3">
         <v>53</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F47" s="3">
         <v>31.34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="48" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
         <v>44370</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B48" s="3">
         <v>204</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C48" s="3">
         <v>40</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D48" s="3">
         <v>75</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E48" s="3">
         <v>89</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F48" s="3">
         <v>19.61</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="49" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>44369</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B49" s="3">
         <v>189</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C49" s="3">
         <v>31</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D49" s="3">
         <v>65</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E49" s="3">
         <v>93</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F49" s="3">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="50" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>44368</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B50" s="3">
         <v>193</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C50" s="3">
         <v>26</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D50" s="3">
         <v>54</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E50" s="3">
         <v>113</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F50" s="3">
         <v>13.47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="51" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
         <v>44367</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B51" s="3">
         <v>168</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C51" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D51" s="3">
         <v>56</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E51" s="3">
         <v>97</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F51" s="3">
         <v>8.93</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="52" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
         <v>44366</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B52" s="3">
         <v>169</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C52" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D52" s="3">
         <v>49</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E52" s="3">
         <v>107</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F52" s="3">
         <v>7.69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="53" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
         <v>44365</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B53" s="3">
         <v>211</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C53" s="3">
         <v>11</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D53" s="3">
         <v>77</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E53" s="3">
         <v>123</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F53" s="3">
         <v>5.21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="54" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
         <v>44364</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B54" s="3">
         <v>230</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C54" s="3">
         <v>21</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D54" s="3">
         <v>92</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E54" s="3">
         <v>117</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F54" s="3">
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="55" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
         <v>44363</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B55" s="3">
         <v>303</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C55" s="3">
         <v>20</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D55" s="3">
         <v>133</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E55" s="3">
         <v>150</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F55" s="3">
         <v>6.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="56" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
         <v>44362</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B56" s="3">
         <v>313</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C56" s="3">
         <v>17</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D56" s="3">
         <v>105</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E56" s="3">
         <v>191</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F56" s="3">
         <v>5.43</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="57" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
         <v>44361</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B57" s="3">
         <v>327</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C57" s="3">
         <v>11</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D57" s="3">
         <v>102</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E57" s="3">
         <v>214</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F57" s="3">
         <v>3.36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="58" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
         <v>44360</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B58" s="3">
         <v>234</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C58" s="3">
         <v>11</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D58" s="3">
         <v>94</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E58" s="3">
         <v>129</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F58" s="3">
         <v>4.7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="59" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
         <v>44359</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B59" s="3">
         <v>268</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C59" s="3">
         <v>10</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D59" s="3">
         <v>100</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E59" s="3">
         <v>158</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F59" s="3">
         <v>3.73</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="60" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
         <v>44358</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B60" s="3">
         <v>355</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C60" s="3">
         <v>5</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D60" s="3">
         <v>134</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E60" s="3">
         <v>216</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F60" s="3">
         <v>1.41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="61" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
         <v>44357</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B61" s="3">
         <v>443</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C61" s="3">
         <v>8</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D61" s="3">
         <v>165</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E61" s="3">
         <v>270</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F61" s="3">
         <v>1.81</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+    <row r="62" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
         <v>44356</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B62" s="3">
         <v>505</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C62" s="3">
         <v>6</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D62" s="3">
         <v>137</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E62" s="3">
         <v>362</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F62" s="3">
         <v>1.19</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+    <row r="63" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
         <v>44355</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B63" s="3">
         <v>541</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C63" s="3">
         <v>9</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D63" s="3">
         <v>142</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E63" s="3">
         <v>390</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F63" s="3">
         <v>1.66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="64" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
         <v>44354</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B64" s="3">
         <v>640</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C64" s="3">
         <v>10</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D64" s="3">
         <v>163</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E64" s="3">
         <v>467</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F64" s="3">
         <v>1.56</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+    <row r="65" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
         <v>44353</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B65" s="3">
         <v>573</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C65" s="3">
         <v>2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D65" s="3">
         <v>147</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E65" s="3">
         <v>424</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F65" s="3">
         <v>0.35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="66" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
         <v>44352</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B66" s="3">
         <v>664</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C66" s="3">
         <v>0</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D66" s="3">
         <v>161</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E66" s="3">
         <v>503</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F66" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+    <row r="67" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
         <v>44351</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B67" s="3">
         <v>759</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C67" s="3">
         <v>2</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D67" s="3">
         <v>165</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E67" s="3">
         <v>592</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F67" s="3">
         <v>0.26</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="68" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
         <v>44350</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B68" s="3">
         <v>777</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C68" s="3">
         <v>0</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D68" s="3">
         <v>172</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E68" s="3">
         <v>605</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F68" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="69" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
         <v>44349</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B69" s="3">
         <v>949</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C69" s="3">
         <v>2</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D69" s="3">
         <v>306</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E69" s="3">
         <v>641</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F69" s="3">
         <v>0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="70" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
         <v>44348</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B70" s="3">
         <v>1113</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C70" s="3">
         <v>0</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D70" s="3">
         <v>413</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E70" s="3">
         <v>700</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F70" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>